<commit_message>
Small edit in the PageForItem
</commit_message>
<xml_diff>
--- a/SEP3/SEP3 Documentation/SecurityAssesment.xlsx
+++ b/SEP3/SEP3 Documentation/SecurityAssesment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIA\SEP3\SEP3\SEP3 Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2F3996D-0AE0-434B-8020-70CF0645C7B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BCB47D-46FF-4E00-9D82-7500CF8B8E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="547" xr2:uid="{EB7C77FA-1E98-46DE-834E-B032266319B4}"/>
   </bookViews>
@@ -629,10 +629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C3FB0A-E88E-4A6E-AE13-C42F0B27C2BC}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +863,7 @@
     <row r="6" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="38" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1119,14 +1122,14 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D0DADD6-E868-4DD1-9FCE-B72B726464C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c9e846d4-087c-4651-a3c4-d5f23daeb6d2"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="13311ecb-8bf6-46d3-a22a-6aff9412df2f"/>
+    <ds:schemaRef ds:uri="c9e846d4-087c-4651-a3c4-d5f23daeb6d2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>